<commit_message>
Ajustes edición tema 2
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado04/guion02/EsqueletoGuion_MA_04_02_CO.xlsx
+++ b/fuentes/contenidos/grado04/guion02/EsqueletoGuion_MA_04_02_CO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="729"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="119">
   <si>
     <t>FICHA</t>
   </si>
@@ -285,9 +285,6 @@
     <t>Practica</t>
   </si>
   <si>
-    <t xml:space="preserve">Practica </t>
-  </si>
-  <si>
     <t>Destacado</t>
   </si>
   <si>
@@ -297,9 +294,6 @@
     <t>Profundiza</t>
   </si>
   <si>
-    <t xml:space="preserve">Texto </t>
-  </si>
-  <si>
     <t>Foto</t>
   </si>
   <si>
@@ -312,9 +306,6 @@
     <t>Recuerda</t>
   </si>
   <si>
-    <t>Representación y orden de números naturales en la recta numérica</t>
-  </si>
-  <si>
     <t>Redondeo de números naturales</t>
   </si>
   <si>
@@ -366,9 +357,6 @@
     <t>Webs de referencia</t>
   </si>
   <si>
-    <t>Descomponer números naturales en posiciones</t>
-  </si>
-  <si>
     <t>Resolver problemas aplicando sustracción de números naturales</t>
   </si>
   <si>
@@ -376,6 +364,30 @@
   </si>
   <si>
     <t>Los números naturales son la base de nuestro sistema de numeración. Conoce sus usos y propiedades, aprende a compararlos y ordenarlos, a redondear y practicar otros sistemas de numeración.</t>
+  </si>
+  <si>
+    <t>Identifica el uso de los números naturales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifica el número natural siguiente </t>
+  </si>
+  <si>
+    <t>Descomposición de números naturales en posiciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Representación y orden de números naturales en la recta numérica </t>
+  </si>
+  <si>
+    <t>Ubicar valores en la recta numérica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redondear – aproximar números naturales </t>
+  </si>
+  <si>
+    <t>Los términos de la división: División exacta e inexacta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Practica la numeración romana </t>
   </si>
 </sst>
 </file>
@@ -1650,7 +1662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1681,7 +1693,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2874,9 +2886,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I113"/>
+  <dimension ref="A1:I115"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H106" sqref="H106"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2887,7 +2901,7 @@
     <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="47.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="83.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2945,18 +2959,14 @@
         <v>19</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
-      <c r="H3" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>23</v>
-      </c>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
@@ -2983,14 +2993,14 @@
         <v>19</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5" s="24"/>
       <c r="E5" s="24"/>
       <c r="F5" s="24"/>
       <c r="G5" s="24"/>
       <c r="H5" s="18" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="I5" s="18" t="s">
         <v>23</v>
@@ -3021,14 +3031,18 @@
         <v>19</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="H7" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
@@ -3037,13 +3051,11 @@
       <c r="B8" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="E8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>82</v>
       </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="24"/>
       <c r="G8" s="24"/>
       <c r="H8" s="18"/>
@@ -3056,21 +3068,15 @@
       <c r="B9" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>87</v>
-      </c>
+      <c r="C9" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
-      <c r="H9" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>23</v>
-      </c>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -3081,10 +3087,10 @@
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
@@ -3100,15 +3106,19 @@
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="24" t="s">
         <v>86</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>89</v>
       </c>
       <c r="F11" s="24"/>
       <c r="G11" s="24"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="H11" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
@@ -3119,10 +3129,10 @@
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F12" s="24"/>
       <c r="G12" s="24"/>
@@ -3138,10 +3148,10 @@
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="F13" s="24"/>
       <c r="G13" s="24"/>
@@ -3157,10 +3167,10 @@
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F14" s="24"/>
       <c r="G14" s="24"/>
@@ -3176,7 +3186,7 @@
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E15" s="24" t="s">
         <v>82</v>
@@ -3195,19 +3205,15 @@
       </c>
       <c r="C16" s="23"/>
       <c r="D16" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F16" s="24"/>
       <c r="G16" s="24"/>
-      <c r="H16" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="I16" s="18" t="s">
-        <v>23</v>
-      </c>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
@@ -3218,19 +3224,15 @@
       </c>
       <c r="C17" s="23"/>
       <c r="D17" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F17" s="24"/>
       <c r="G17" s="24"/>
-      <c r="H17" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="I17" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
@@ -3241,15 +3243,19 @@
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F18" s="24"/>
       <c r="G18" s="24"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
+      <c r="H18" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
@@ -3260,15 +3266,19 @@
       </c>
       <c r="C19" s="23"/>
       <c r="D19" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="24" t="s">
         <v>86</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>85</v>
       </c>
       <c r="F19" s="24"/>
       <c r="G19" s="24"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
+      <c r="H19" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
@@ -3279,7 +3289,7 @@
       </c>
       <c r="C20" s="23"/>
       <c r="D20" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E20" s="24" t="s">
         <v>82</v>
@@ -3298,10 +3308,10 @@
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F21" s="24"/>
       <c r="G21" s="24"/>
@@ -3317,19 +3327,15 @@
       </c>
       <c r="C22" s="23"/>
       <c r="D22" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F22" s="24"/>
       <c r="G22" s="24"/>
-      <c r="H22" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I22" s="18" t="s">
-        <v>23</v>
-      </c>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
@@ -3340,10 +3346,10 @@
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="24" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="F23" s="24"/>
       <c r="G23" s="24"/>
@@ -3359,15 +3365,19 @@
       </c>
       <c r="C24" s="23"/>
       <c r="D24" s="24" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
+      <c r="H24" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
@@ -3378,7 +3388,7 @@
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E25" s="24" t="s">
         <v>82</v>
@@ -3396,11 +3406,11 @@
         <v>19</v>
       </c>
       <c r="C26" s="25"/>
-      <c r="D26" s="26" t="s">
-        <v>90</v>
+      <c r="D26" s="24" t="s">
+        <v>88</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F26" s="26"/>
       <c r="G26" s="26"/>
@@ -3415,20 +3425,16 @@
         <v>19</v>
       </c>
       <c r="C27" s="25"/>
-      <c r="D27" s="26" t="s">
-        <v>90</v>
+      <c r="D27" s="24" t="s">
+        <v>88</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F27" s="26"/>
       <c r="G27" s="26"/>
-      <c r="H27" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="H27" s="15"/>
+      <c r="I27" s="18"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
@@ -3438,8 +3444,8 @@
         <v>19</v>
       </c>
       <c r="C28" s="25"/>
-      <c r="D28" s="26" t="s">
-        <v>90</v>
+      <c r="D28" s="24" t="s">
+        <v>88</v>
       </c>
       <c r="E28" s="26" t="s">
         <v>83</v>
@@ -3447,7 +3453,7 @@
       <c r="F28" s="26"/>
       <c r="G28" s="26"/>
       <c r="H28" s="15" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="I28" s="18" t="s">
         <v>25</v>
@@ -3461,16 +3467,20 @@
         <v>19</v>
       </c>
       <c r="C29" s="25"/>
-      <c r="D29" s="26" t="s">
-        <v>91</v>
+      <c r="D29" s="24" t="s">
+        <v>88</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F29" s="26"/>
       <c r="G29" s="26"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="18"/>
+      <c r="H29" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
@@ -3481,10 +3491,10 @@
       </c>
       <c r="C30" s="25"/>
       <c r="D30" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F30" s="26"/>
       <c r="G30" s="26"/>
@@ -3500,10 +3510,10 @@
       </c>
       <c r="C31" s="25"/>
       <c r="D31" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F31" s="26"/>
       <c r="G31" s="26"/>
@@ -3519,10 +3529,10 @@
       </c>
       <c r="C32" s="25"/>
       <c r="D32" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F32" s="26"/>
       <c r="G32" s="26"/>
@@ -3538,7 +3548,7 @@
       </c>
       <c r="C33" s="25"/>
       <c r="D33" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E33" s="26" t="s">
         <v>82</v>
@@ -3557,19 +3567,15 @@
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F34" s="26"/>
       <c r="G34" s="26"/>
-      <c r="H34" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="I34" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="H34" s="15"/>
+      <c r="I34" s="18"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
@@ -3580,19 +3586,15 @@
       </c>
       <c r="C35" s="25"/>
       <c r="D35" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F35" s="26"/>
       <c r="G35" s="26"/>
-      <c r="H35" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="I35" s="18" t="s">
-        <v>23</v>
-      </c>
+      <c r="H35" s="15"/>
+      <c r="I35" s="18"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
@@ -3603,15 +3605,19 @@
       </c>
       <c r="C36" s="25"/>
       <c r="D36" s="26" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F36" s="26"/>
       <c r="G36" s="26"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="18"/>
+      <c r="H36" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I36" s="18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
@@ -3622,15 +3628,19 @@
       </c>
       <c r="C37" s="25"/>
       <c r="D37" s="26" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F37" s="26"/>
       <c r="G37" s="26"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="18"/>
+      <c r="H37" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="I37" s="18" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
@@ -3641,7 +3651,7 @@
       </c>
       <c r="C38" s="25"/>
       <c r="D38" s="26" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="E38" s="26" t="s">
         <v>82</v>
@@ -3660,19 +3670,15 @@
       </c>
       <c r="C39" s="25"/>
       <c r="D39" s="26" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F39" s="26"/>
       <c r="G39" s="26"/>
-      <c r="H39" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="I39" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="H39" s="15"/>
+      <c r="I39" s="18"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
@@ -3683,19 +3689,15 @@
       </c>
       <c r="C40" s="25"/>
       <c r="D40" s="26" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F40" s="26"/>
       <c r="G40" s="26"/>
-      <c r="H40" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="I40" s="18" t="s">
-        <v>23</v>
-      </c>
+      <c r="H40" s="15"/>
+      <c r="I40" s="18"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
@@ -3706,7 +3708,7 @@
       </c>
       <c r="C41" s="25"/>
       <c r="D41" s="26" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="E41" s="26" t="s">
         <v>83</v>
@@ -3714,10 +3716,10 @@
       <c r="F41" s="26"/>
       <c r="G41" s="26"/>
       <c r="H41" s="15" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="I41" s="18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3729,15 +3731,19 @@
       </c>
       <c r="C42" s="25"/>
       <c r="D42" s="26" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F42" s="26"/>
       <c r="G42" s="26"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="18"/>
+      <c r="H42" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="I42" s="18" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
@@ -3748,15 +3754,19 @@
       </c>
       <c r="C43" s="25"/>
       <c r="D43" s="26" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F43" s="26"/>
       <c r="G43" s="26"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="18"/>
+      <c r="H43" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I43" s="18" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
@@ -3767,7 +3777,7 @@
       </c>
       <c r="C44" s="25"/>
       <c r="D44" s="26" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E44" s="26" t="s">
         <v>82</v>
@@ -3786,10 +3796,10 @@
       </c>
       <c r="C45" s="25"/>
       <c r="D45" s="26" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E45" s="26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
@@ -3805,10 +3815,10 @@
       </c>
       <c r="C46" s="25"/>
       <c r="D46" s="26" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E46" s="26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F46" s="26"/>
       <c r="G46" s="26"/>
@@ -3824,7 +3834,7 @@
       </c>
       <c r="C47" s="25"/>
       <c r="D47" s="26" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E47" s="26" t="s">
         <v>83</v>
@@ -3832,7 +3842,7 @@
       <c r="F47" s="26"/>
       <c r="G47" s="26"/>
       <c r="H47" s="15" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="I47" s="18" t="s">
         <v>25</v>
@@ -3847,7 +3857,7 @@
       </c>
       <c r="C48" s="25"/>
       <c r="D48" s="26" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E48" s="26" t="s">
         <v>82</v>
@@ -3866,7 +3876,7 @@
       </c>
       <c r="C49" s="25"/>
       <c r="D49" s="26" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E49" s="26" t="s">
         <v>83</v>
@@ -3885,7 +3895,7 @@
         <v>19</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C50" s="25" t="s">
         <v>82</v>
@@ -3902,11 +3912,11 @@
         <v>19</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C51" s="25"/>
       <c r="D51" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E51" s="26" t="s">
         <v>82</v>
@@ -3921,14 +3931,14 @@
         <v>19</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C52" s="25"/>
       <c r="D52" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E52" s="26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F52" s="26"/>
       <c r="G52" s="26"/>
@@ -3940,18 +3950,18 @@
         <v>19</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C53" s="25"/>
       <c r="D53" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E53" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F53" s="26"/>
       <c r="G53" s="26"/>
-      <c r="H53" s="15" t="s">
+      <c r="H53" s="7" t="s">
         <v>50</v>
       </c>
       <c r="I53" s="18" t="s">
@@ -3963,11 +3973,11 @@
         <v>19</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C54" s="25"/>
       <c r="D54" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E54" s="26" t="s">
         <v>83</v>
@@ -3986,15 +3996,15 @@
         <v>19</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C55" s="25"/>
       <c r="D55" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E55" s="26"/>
       <c r="F55" s="26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G55" s="26" t="s">
         <v>82</v>
@@ -4007,18 +4017,18 @@
         <v>19</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C56" s="25"/>
       <c r="D56" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E56" s="26"/>
       <c r="F56" s="26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G56" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H56" s="15"/>
       <c r="I56" s="18"/>
@@ -4028,15 +4038,15 @@
         <v>19</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C57" s="25"/>
       <c r="D57" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E57" s="26"/>
       <c r="F57" s="26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G57" s="26" t="s">
         <v>82</v>
@@ -4049,18 +4059,18 @@
         <v>19</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C58" s="25"/>
       <c r="D58" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E58" s="26"/>
       <c r="F58" s="26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G58" s="26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H58" s="15"/>
       <c r="I58" s="18"/>
@@ -4070,15 +4080,15 @@
         <v>19</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C59" s="25"/>
       <c r="D59" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E59" s="26"/>
       <c r="F59" s="26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G59" s="26" t="s">
         <v>82</v>
@@ -4091,18 +4101,18 @@
         <v>19</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C60" s="25"/>
       <c r="D60" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E60" s="26"/>
       <c r="F60" s="26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G60" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H60" s="15"/>
       <c r="I60" s="18"/>
@@ -4112,15 +4122,15 @@
         <v>19</v>
       </c>
       <c r="B61" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C61" s="25"/>
       <c r="D61" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E61" s="26"/>
       <c r="F61" s="26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G61" s="26" t="s">
         <v>82</v>
@@ -4133,18 +4143,18 @@
         <v>19</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C62" s="25"/>
       <c r="D62" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E62" s="26"/>
       <c r="F62" s="26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G62" s="26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H62" s="15"/>
       <c r="I62" s="18"/>
@@ -4154,15 +4164,15 @@
         <v>19</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C63" s="25"/>
       <c r="D63" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E63" s="26"/>
       <c r="F63" s="26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G63" s="26" t="s">
         <v>82</v>
@@ -4175,18 +4185,18 @@
         <v>19</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C64" s="25"/>
       <c r="D64" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E64" s="26"/>
       <c r="F64" s="26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G64" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H64" s="15"/>
       <c r="I64" s="18"/>
@@ -4196,15 +4206,15 @@
         <v>19</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C65" s="25"/>
       <c r="D65" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E65" s="26"/>
       <c r="F65" s="26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G65" s="26" t="s">
         <v>83</v>
@@ -4221,11 +4231,11 @@
         <v>19</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C66" s="25"/>
       <c r="D66" s="26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E66" s="26" t="s">
         <v>82</v>
@@ -4240,14 +4250,14 @@
         <v>19</v>
       </c>
       <c r="B67" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C67" s="25"/>
       <c r="D67" s="26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E67" s="26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F67" s="26"/>
       <c r="G67" s="26"/>
@@ -4259,14 +4269,14 @@
         <v>19</v>
       </c>
       <c r="B68" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C68" s="25"/>
       <c r="D68" s="26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E68" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F68" s="26"/>
       <c r="G68" s="26"/>
@@ -4282,11 +4292,11 @@
         <v>19</v>
       </c>
       <c r="B69" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C69" s="25"/>
       <c r="D69" s="26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E69" s="26" t="s">
         <v>83</v>
@@ -4294,7 +4304,7 @@
       <c r="F69" s="26"/>
       <c r="G69" s="26"/>
       <c r="H69" s="15" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I69" s="18" t="s">
         <v>23</v>
@@ -4305,11 +4315,11 @@
         <v>19</v>
       </c>
       <c r="B70" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C70" s="25"/>
       <c r="D70" s="26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E70" s="26" t="s">
         <v>82</v>
@@ -4324,14 +4334,14 @@
         <v>19</v>
       </c>
       <c r="B71" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C71" s="25"/>
       <c r="D71" s="26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E71" s="26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F71" s="26"/>
       <c r="G71" s="26"/>
@@ -4343,14 +4353,14 @@
         <v>19</v>
       </c>
       <c r="B72" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C72" s="25"/>
       <c r="D72" s="26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E72" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F72" s="26"/>
       <c r="G72" s="26"/>
@@ -4366,38 +4376,36 @@
         <v>19</v>
       </c>
       <c r="B73" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C73" s="25"/>
       <c r="D73" s="26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E73" s="26" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F73" s="26"/>
       <c r="G73" s="26"/>
       <c r="H73" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="I73" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="I73" s="18"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B74" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C74" s="25"/>
       <c r="D74" s="26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E74" s="26"/>
       <c r="F74" s="26" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G74" s="26" t="s">
         <v>82</v>
@@ -4410,18 +4418,18 @@
         <v>19</v>
       </c>
       <c r="B75" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C75" s="25"/>
       <c r="D75" s="26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E75" s="26"/>
       <c r="F75" s="26" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G75" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H75" s="15" t="s">
         <v>58</v>
@@ -4435,18 +4443,18 @@
         <v>19</v>
       </c>
       <c r="B76" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C76" s="25"/>
       <c r="D76" s="26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E76" s="26"/>
       <c r="F76" s="26" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G76" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H76" s="15" t="s">
         <v>59</v>
@@ -4460,11 +4468,11 @@
         <v>19</v>
       </c>
       <c r="B77" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C77" s="25"/>
       <c r="D77" s="26" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E77" s="26" t="s">
         <v>82</v>
@@ -4479,14 +4487,14 @@
         <v>19</v>
       </c>
       <c r="B78" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C78" s="25"/>
       <c r="D78" s="26" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E78" s="26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F78" s="26"/>
       <c r="G78" s="26"/>
@@ -4498,14 +4506,14 @@
         <v>19</v>
       </c>
       <c r="B79" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C79" s="25"/>
       <c r="D79" s="26" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E79" s="26" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F79" s="26"/>
       <c r="G79" s="26"/>
@@ -4517,14 +4525,14 @@
         <v>19</v>
       </c>
       <c r="B80" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C80" s="25"/>
       <c r="D80" s="26" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E80" s="26" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F80" s="26"/>
       <c r="G80" s="26"/>
@@ -4536,95 +4544,95 @@
         <v>19</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C81" s="25"/>
       <c r="D81" s="26" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E81" s="26" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F81" s="26"/>
       <c r="G81" s="26"/>
-      <c r="H81" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="I81" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="H81" s="15"/>
+      <c r="I81" s="18"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B82" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C82" s="25"/>
       <c r="D82" s="26" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E82" s="26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F82" s="26"/>
       <c r="G82" s="26"/>
-      <c r="H82" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I82" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="H82" s="15"/>
+      <c r="I82" s="18"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B83" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C83" s="25"/>
       <c r="D83" s="26" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E83" s="26" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F83" s="26"/>
       <c r="G83" s="26"/>
-      <c r="H83" s="15"/>
-      <c r="I83" s="18"/>
+      <c r="H83" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="I83" s="18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B84" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C84" s="25"/>
       <c r="D84" s="26" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E84" s="26" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F84" s="26"/>
       <c r="G84" s="26"/>
-      <c r="H84" s="15"/>
-      <c r="I84" s="18"/>
+      <c r="H84" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="I84" s="18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B85" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C85" s="25"/>
       <c r="D85" s="26" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E85" s="26" t="s">
         <v>82</v>
@@ -4639,68 +4647,60 @@
         <v>19</v>
       </c>
       <c r="B86" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C86" s="25"/>
       <c r="D86" s="26" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E86" s="26" t="s">
         <v>87</v>
       </c>
       <c r="F86" s="26"/>
       <c r="G86" s="26"/>
-      <c r="H86" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I86" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="H86" s="15"/>
+      <c r="I86" s="18"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C87" s="25"/>
       <c r="D87" s="26" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E87" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F87" s="26"/>
       <c r="G87" s="26"/>
-      <c r="H87" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="I87" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="H87" s="15"/>
+      <c r="I87" s="18"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B88" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C88" s="25"/>
       <c r="D88" s="26" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E88" s="26" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F88" s="26"/>
       <c r="G88" s="26"/>
       <c r="H88" s="15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I88" s="18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -4708,49 +4708,57 @@
         <v>19</v>
       </c>
       <c r="B89" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C89" s="25"/>
       <c r="D89" s="26" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E89" s="26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F89" s="26"/>
       <c r="G89" s="26"/>
-      <c r="H89" s="15"/>
-      <c r="I89" s="18"/>
+      <c r="H89" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I89" s="18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B90" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C90" s="25"/>
       <c r="D90" s="26" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E90" s="26" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F90" s="26"/>
       <c r="G90" s="26"/>
-      <c r="H90" s="15"/>
-      <c r="I90" s="18"/>
+      <c r="H90" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="I90" s="18" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B91" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C91" s="25"/>
       <c r="D91" s="26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E91" s="26" t="s">
         <v>82</v>
@@ -4765,14 +4773,14 @@
         <v>19</v>
       </c>
       <c r="B92" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C92" s="25"/>
       <c r="D92" s="26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E92" s="26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F92" s="26"/>
       <c r="G92" s="26"/>
@@ -4784,37 +4792,33 @@
         <v>19</v>
       </c>
       <c r="B93" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C93" s="25"/>
       <c r="D93" s="26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E93" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F93" s="26"/>
       <c r="G93" s="26"/>
-      <c r="H93" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="I93" s="18" t="s">
-        <v>23</v>
-      </c>
+      <c r="H93" s="15"/>
+      <c r="I93" s="18"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B94" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C94" s="25"/>
       <c r="D94" s="26" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="E94" s="26" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="F94" s="26"/>
       <c r="G94" s="26"/>
@@ -4826,11 +4830,11 @@
         <v>19</v>
       </c>
       <c r="B95" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C95" s="25"/>
       <c r="D95" s="26" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="E95" s="26" t="s">
         <v>83</v>
@@ -4838,10 +4842,10 @@
       <c r="F95" s="26"/>
       <c r="G95" s="26"/>
       <c r="H95" s="15" t="s">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="I95" s="18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -4849,13 +4853,15 @@
         <v>19</v>
       </c>
       <c r="B96" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="C96" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C96" s="25"/>
+      <c r="D96" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E96" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="D96" s="26"/>
-      <c r="E96" s="26"/>
       <c r="F96" s="26"/>
       <c r="G96" s="26"/>
       <c r="H96" s="15"/>
@@ -4866,34 +4872,36 @@
         <v>19</v>
       </c>
       <c r="B97" s="23" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C97" s="25"/>
       <c r="D97" s="26" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="E97" s="26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F97" s="26"/>
       <c r="G97" s="26"/>
-      <c r="H97" s="15"/>
-      <c r="I97" s="18"/>
+      <c r="H97" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="I97" s="18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B98" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="C98" s="25"/>
-      <c r="D98" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="E98" s="26" t="s">
-        <v>89</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="C98" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D98" s="26"/>
+      <c r="E98" s="26"/>
       <c r="F98" s="26"/>
       <c r="G98" s="26"/>
       <c r="H98" s="15"/>
@@ -4904,11 +4912,11 @@
         <v>19</v>
       </c>
       <c r="B99" s="23" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C99" s="25"/>
       <c r="D99" s="26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E99" s="26" t="s">
         <v>82</v>
@@ -4923,14 +4931,14 @@
         <v>19</v>
       </c>
       <c r="B100" s="23" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C100" s="25"/>
       <c r="D100" s="26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E100" s="26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F100" s="26"/>
       <c r="G100" s="26"/>
@@ -4942,37 +4950,33 @@
         <v>19</v>
       </c>
       <c r="B101" s="23" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C101" s="25"/>
       <c r="D101" s="26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E101" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F101" s="26"/>
       <c r="G101" s="26"/>
-      <c r="H101" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="I101" s="18" t="s">
-        <v>23</v>
-      </c>
+      <c r="H101" s="15"/>
+      <c r="I101" s="18"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B102" s="23" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C102" s="25"/>
       <c r="D102" s="26" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E102" s="26" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="F102" s="26"/>
       <c r="G102" s="26"/>
@@ -4984,30 +4988,34 @@
         <v>19</v>
       </c>
       <c r="B103" s="23" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C103" s="25"/>
       <c r="D103" s="26" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E103" s="26" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F103" s="26"/>
       <c r="G103" s="26"/>
-      <c r="H103" s="15"/>
-      <c r="I103" s="18"/>
+      <c r="H103" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="I103" s="18" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B104" s="23" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C104" s="25"/>
       <c r="D104" s="26" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E104" s="26" t="s">
         <v>82</v>
@@ -5022,57 +5030,49 @@
         <v>19</v>
       </c>
       <c r="B105" s="23" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C105" s="25"/>
       <c r="D105" s="26" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E105" s="26" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F105" s="26"/>
       <c r="G105" s="26"/>
-      <c r="H105" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="I105" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="H105" s="15"/>
+      <c r="I105" s="18"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B106" s="23" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C106" s="25"/>
       <c r="D106" s="26" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="E106" s="26" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F106" s="26"/>
       <c r="G106" s="26"/>
-      <c r="H106" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="I106" s="18" t="s">
-        <v>23</v>
-      </c>
+      <c r="H106" s="15"/>
+      <c r="I106" s="18"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B107" s="23" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C107" s="25"/>
       <c r="D107" s="26" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="E107" s="26" t="s">
         <v>83</v>
@@ -5080,7 +5080,7 @@
       <c r="F107" s="26"/>
       <c r="G107" s="26"/>
       <c r="H107" s="15" t="s">
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="I107" s="18" t="s">
         <v>25</v>
@@ -5091,37 +5091,45 @@
         <v>19</v>
       </c>
       <c r="B108" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="C108" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="D108" s="26"/>
-      <c r="E108" s="26"/>
+        <v>102</v>
+      </c>
+      <c r="C108" s="25"/>
+      <c r="D108" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E108" s="26" t="s">
+        <v>86</v>
+      </c>
       <c r="F108" s="26"/>
       <c r="G108" s="26"/>
-      <c r="H108" s="15"/>
-      <c r="I108" s="18"/>
+      <c r="H108" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="I108" s="18" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B109" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="C109" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C109" s="25"/>
+      <c r="D109" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E109" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="D109" s="26"/>
-      <c r="E109" s="26"/>
       <c r="F109" s="26"/>
       <c r="G109" s="26"/>
       <c r="H109" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I109" s="18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -5129,55 +5137,55 @@
         <v>19</v>
       </c>
       <c r="B110" s="23" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C110" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D110" s="26"/>
       <c r="E110" s="26"/>
       <c r="F110" s="26"/>
       <c r="G110" s="26"/>
-      <c r="H110" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="I110" s="18" t="s">
-        <v>23</v>
-      </c>
+      <c r="H110" s="15"/>
+      <c r="I110" s="18"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B111" s="23" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C111" s="25" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D111" s="26"/>
       <c r="E111" s="26"/>
       <c r="F111" s="26"/>
       <c r="G111" s="26"/>
-      <c r="H111" s="15"/>
-      <c r="I111" s="18"/>
+      <c r="H111" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="I111" s="18" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B112" s="23" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C112" s="25" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D112" s="26"/>
       <c r="E112" s="26"/>
       <c r="F112" s="26"/>
       <c r="G112" s="26"/>
       <c r="H112" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I112" s="18" t="s">
         <v>23</v>
@@ -5188,10 +5196,10 @@
         <v>19</v>
       </c>
       <c r="B113" s="23" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C113" s="25" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="D113" s="26"/>
       <c r="E113" s="26"/>
@@ -5200,9 +5208,47 @@
       <c r="H113" s="15"/>
       <c r="I113" s="18"/>
     </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B114" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C114" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D114" s="26"/>
+      <c r="E114" s="26"/>
+      <c r="F114" s="26"/>
+      <c r="G114" s="26"/>
+      <c r="H114" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="I114" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B115" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C115" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D115" s="26"/>
+      <c r="E115" s="26"/>
+      <c r="F115" s="26"/>
+      <c r="G115" s="26"/>
+      <c r="H115" s="15"/>
+      <c r="I115" s="18"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>